<commit_message>
add gitPathProject for files
</commit_message>
<xml_diff>
--- a/cypress-framework/cypress/fixtures/ContactFormTestCase.xlsx
+++ b/cypress-framework/cypress/fixtures/ContactFormTestCase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation Test\Cypress\cypress-framework\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Radu\Documents\GitHub\ProjectAssistHomework\cypress-framework\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{39B739A8-5BE2-4D95-B84A-5315CA63D1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4594AF1D-7C9C-4D9D-947A-594AFFB8BFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="648" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Textbox Name" sheetId="1" r:id="rId1"/>
@@ -332,9 +332,6 @@
     <t xml:space="preserve">All required fields are empty </t>
   </si>
   <si>
-    <t>1)Click on Experience field      2)Select 1-3      3)Click on Submit</t>
-  </si>
-  <si>
     <t xml:space="preserve"> '1-3' </t>
   </si>
   <si>
@@ -362,9 +359,6 @@
     <t xml:space="preserve">All required fields are filled </t>
   </si>
   <si>
-    <t>1)Click on Experience field      2)Select 5-7      3)Click on Submit</t>
-  </si>
-  <si>
     <t xml:space="preserve"> '5-7' </t>
   </si>
   <si>
@@ -482,15 +476,6 @@
     <t xml:space="preserve">Comment field cannot be empty </t>
   </si>
   <si>
-    <t xml:space="preserve">1)Click on Comment field      2)Click Submit </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1)Click on Comment field        2)Press space button       3)Click Submit </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1)Click on Comment field       2)Type Lorem ipsum      3)Click on Submit </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 'Lorem ipsum' </t>
   </si>
   <si>
@@ -755,9 +740,6 @@
     <t xml:space="preserve"> Values are equal</t>
   </si>
   <si>
-    <t xml:space="preserve"> pass </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Verify checkbox "Expertise"</t>
   </si>
   <si>
@@ -797,9 +779,6 @@
     <t xml:space="preserve"> The button color is rgb(68; 68; 68)</t>
   </si>
   <si>
-    <t xml:space="preserve"> pass  </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Verify hover color on button ALERT BOX</t>
   </si>
   <si>
@@ -899,7 +878,28 @@
     <t xml:space="preserve">1)Click on Choose File      2)Select from fixtures photoS.jpg      3)Click Submit </t>
   </si>
   <si>
-    <t xml:space="preserve"> pass</t>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>1)Click on Experience field      2)Select 1-3                             3)Click on Submit</t>
+  </si>
+  <si>
+    <t>1)Click on Experience field      2)Select 5-7                           3)Click on Submit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Click on Comment field       2)Click Submit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Click on Comment field        2)Press space button                    3)Click Submit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Click on Comment field       2)Type Lorem ipsum                  3)Click on Submit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Click on Comment field          2)Click Submit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Click on Comment field       2)Type Lorem ipsum                    3)Click on Submit </t>
   </si>
 </sst>
 </file>
@@ -1008,21 +1008,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -2145,18 +2131,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I1048576">
-    <cfRule type="containsText" dxfId="15" priority="4" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="5" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"fail"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2169,15 +2155,16 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927749FA-E2DC-4C2A-8050-BEF3100D8D9E}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="5" width="29.5703125" customWidth="1"/>
     <col min="6" max="6" width="40.42578125" customWidth="1"/>
     <col min="7" max="7" width="41.5703125" customWidth="1"/>
@@ -2243,7 +2230,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30">
+    <row r="3" spans="1:9" ht="45">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -2266,7 +2253,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="I3" s="13" t="s">
         <v>33</v>
@@ -2301,7 +2288,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45">
+    <row r="5" spans="1:9" ht="60">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -2330,7 +2317,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="45">
+    <row r="6" spans="1:9" ht="60">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -2359,7 +2346,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45">
+    <row r="7" spans="1:9" ht="60">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -2417,7 +2404,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30">
+    <row r="9" spans="1:9" ht="45">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -2440,7 +2427,7 @@
         <v>26</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>33</v>
@@ -2533,7 +2520,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="45">
+    <row r="13" spans="1:9" ht="60">
       <c r="A13" s="13">
         <v>12</v>
       </c>
@@ -2564,10 +2551,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"fail"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2589,7 +2576,7 @@
     <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.5703125" customWidth="1"/>
     <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="34.42578125" customWidth="1"/>
     <col min="6" max="6" width="40.85546875" customWidth="1"/>
     <col min="7" max="7" width="40.5703125" customWidth="1"/>
@@ -2655,7 +2642,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30">
+    <row r="3" spans="1:9" ht="45">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -2684,7 +2671,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30">
+    <row r="4" spans="1:9" ht="45">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -2713,7 +2700,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30">
+    <row r="5" spans="1:9" ht="60">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -2742,7 +2729,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="45">
+    <row r="6" spans="1:9" ht="60">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -2800,7 +2787,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30">
+    <row r="8" spans="1:9" ht="45">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -2829,7 +2816,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30">
+    <row r="9" spans="1:9" ht="45">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -2858,7 +2845,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30">
+    <row r="10" spans="1:9" ht="60">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -2887,7 +2874,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="45">
+    <row r="11" spans="1:9" ht="60">
       <c r="A11" s="13">
         <v>10</v>
       </c>
@@ -2945,7 +2932,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30">
+    <row r="13" spans="1:9" ht="45">
       <c r="A13" s="13">
         <v>12</v>
       </c>
@@ -2974,7 +2961,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30">
+    <row r="14" spans="1:9" ht="45">
       <c r="A14" s="13" t="s">
         <v>81</v>
       </c>
@@ -3003,7 +2990,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30">
+    <row r="15" spans="1:9" ht="45">
       <c r="A15" s="13">
         <v>13</v>
       </c>
@@ -3032,7 +3019,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30">
+    <row r="16" spans="1:9" ht="60">
       <c r="A16" s="13">
         <v>14</v>
       </c>
@@ -3061,7 +3048,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="45">
+    <row r="17" spans="1:9" ht="60">
       <c r="A17" s="13">
         <v>15</v>
       </c>
@@ -3092,10 +3079,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3109,14 +3096,14 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
     <col min="2" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
     <col min="5" max="5" width="29.5703125" customWidth="1"/>
     <col min="6" max="6" width="40.42578125" customWidth="1"/>
     <col min="7" max="7" width="41.5703125" customWidth="1"/>
@@ -3153,7 +3140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30">
+    <row r="2" spans="1:9" ht="45">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3164,10 +3151,10 @@
         <v>98</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>11</v>
@@ -3187,22 +3174,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>13</v>
@@ -3211,27 +3198,27 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30">
+    <row r="4" spans="1:9" ht="45">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>13</v>
@@ -3245,16 +3232,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>98</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>11</v>
@@ -3274,22 +3261,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>13</v>
@@ -3303,22 +3290,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>13</v>
@@ -3332,16 +3319,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>98</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>11</v>
@@ -3361,22 +3348,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>13</v>
@@ -3390,22 +3377,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>13</v>
@@ -3416,10 +3403,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"fail"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3431,15 +3418,15 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B9D747E-30CB-4DE6-8F77-E32E0F1DF2EC}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
     <col min="2" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1"/>
     <col min="5" max="5" width="29.5703125" customWidth="1"/>
     <col min="6" max="6" width="40.42578125" customWidth="1"/>
     <col min="7" max="7" width="41.5703125" customWidth="1"/>
@@ -3481,22 +3468,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>98</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>138</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>140</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>13</v>
@@ -3510,22 +3497,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>144</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>13</v>
@@ -3539,22 +3526,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>138</v>
-      </c>
       <c r="F4" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>13</v>
@@ -3568,13 +3555,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>149</v>
+        <v>284</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>10</v>
@@ -3597,13 +3584,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>150</v>
+        <v>285</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>16</v>
@@ -3621,21 +3608,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30">
+    <row r="7" spans="1:9" ht="45">
       <c r="A7" s="13">
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>151</v>
+        <v>286</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>11</v>
@@ -3655,22 +3642,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>13</v>
@@ -3684,19 +3671,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>149</v>
+        <v>287</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>78</v>
@@ -3713,22 +3700,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>150</v>
+        <v>285</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>13</v>
@@ -3737,27 +3724,27 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30">
+    <row r="11" spans="1:9" ht="45">
       <c r="A11" s="13">
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>151</v>
+        <v>288</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>13</v>
@@ -3771,22 +3758,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>98</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>13</v>
@@ -3800,22 +3787,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C13" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F13" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>143</v>
-      </c>
       <c r="G13" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>13</v>
@@ -3829,22 +3816,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F14" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>167</v>
-      </c>
       <c r="G14" s="13" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="H14" s="13" t="s">
         <v>13</v>
@@ -3855,10 +3842,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3870,8 +3857,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FADFCE-49FC-4DFD-A36B-AF33F3184472}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3922,28 +3909,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>174</v>
-      </c>
       <c r="I2" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="45">
@@ -3951,28 +3938,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45">
@@ -3980,28 +3967,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45">
@@ -4009,28 +3996,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="45">
@@ -4038,28 +4025,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45">
@@ -4067,28 +4054,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="H7" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="45">
@@ -4096,28 +4083,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="H8" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="45">
@@ -4125,28 +4112,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="H9" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45">
@@ -4154,28 +4141,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45">
@@ -4183,28 +4170,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="45">
@@ -4212,28 +4199,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45">
@@ -4241,28 +4228,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="45">
@@ -4270,28 +4257,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45">
@@ -4299,28 +4286,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>202</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="45">
@@ -4328,28 +4315,28 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="45">
@@ -4357,28 +4344,28 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="45">
@@ -4386,28 +4373,28 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="45">
@@ -4415,28 +4402,28 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="45">
@@ -4444,28 +4431,28 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="F20" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="45">
@@ -4473,28 +4460,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45">
@@ -4502,28 +4489,28 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="45">
@@ -4531,28 +4518,28 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="45">
@@ -4560,28 +4547,28 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="45">
@@ -4589,28 +4576,28 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="45">
@@ -4618,28 +4605,28 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="45">
@@ -4647,28 +4634,28 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="45">
@@ -4676,28 +4663,28 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="D28" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>222</v>
-      </c>
       <c r="F28" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="45">
@@ -4705,28 +4692,28 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="D29" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="45">
@@ -4734,28 +4721,28 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="45">
@@ -4763,28 +4750,28 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>225</v>
-      </c>
       <c r="F31" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="45">
@@ -4792,28 +4779,28 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="45">
@@ -4821,28 +4808,28 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="D33" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="45">
@@ -4850,28 +4837,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="45">
@@ -4879,28 +4866,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="45">
@@ -4908,28 +4895,28 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="30">
@@ -4937,28 +4924,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>239</v>
-      </c>
       <c r="H37" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>240</v>
+        <v>281</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="45">
@@ -4966,28 +4953,28 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>240</v>
+        <v>281</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="30">
@@ -4995,28 +4982,28 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>240</v>
+        <v>281</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="30">
@@ -5024,28 +5011,28 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>254</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="30">
@@ -5053,28 +5040,28 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>256</v>
-      </c>
       <c r="E41" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>240</v>
+        <v>281</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="30">
@@ -5082,28 +5069,28 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>240</v>
+        <v>281</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="30">
@@ -5111,28 +5098,28 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="45">
@@ -5140,28 +5127,28 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="45">
@@ -5169,28 +5156,28 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="45">
@@ -5198,28 +5185,28 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="45">
@@ -5227,28 +5214,28 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="30">
@@ -5256,28 +5243,28 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>254</v>
+        <v>281</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="30">
@@ -5285,28 +5272,28 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>240</v>
+        <v>281</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="45">
@@ -5314,28 +5301,28 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>240</v>
+        <v>281</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="75">
@@ -5343,28 +5330,28 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="I51" s="3" t="s">
         <v>281</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="45">
@@ -5372,13 +5359,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>86</v>
@@ -5398,13 +5385,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>